<commit_message>
Initial setup of Angular application - import of Excel-file and generation of some elements is working at this point.
</commit_message>
<xml_diff>
--- a/Data/icetest-liste.xlsx
+++ b/Data/icetest-liste.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ah\Documents\MED6-Icehorse-Scheduling-Assistant\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumenter\MED6-Icehorse-Scheduling-Assistant\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -3516,48 +3516,48 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="20 % - Farve1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Farve2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Farve3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Farve4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Farve5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Farve6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Farve1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Farve2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Farve3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Farve4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Farve5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Farve6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Farve1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Farve2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Farve3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Farve4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Farve5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Farve6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Advarselstekst" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Bemærk!" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Beregning" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Farve1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Farve2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Farve3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Farve4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Farve5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Farve6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Forklarende tekst" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="God" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Kontrollér celle" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Overskrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Overskrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Overskrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Overskrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Sammenkædet celle" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Titel" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Ugyldig" xfId="7" builtinId="27" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3573,9 +3573,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kontor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3613,7 +3613,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kontor">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3719,7 +3719,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kontor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3871,7 +3871,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O256"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -4031,6 +4033,9 @@
       <c r="G5" t="s">
         <v>32</v>
       </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
       <c r="M5">
         <v>1</v>
       </c>
@@ -4057,6 +4062,9 @@
       <c r="G6" t="s">
         <v>34</v>
       </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
       <c r="O6" t="s">
         <v>20</v>
       </c>
@@ -4086,9 +4094,6 @@
       <c r="H7">
         <v>1</v>
       </c>
-      <c r="L7">
-        <v>1</v>
-      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -4113,9 +4118,6 @@
         <v>44</v>
       </c>
       <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="L8">
         <v>1</v>
       </c>
     </row>

</xml_diff>